<commit_message>
OPSK-1993 fix to spelling typo in sample template
</commit_message>
<xml_diff>
--- a/config/default_data/master-template.xlsx
+++ b/config/default_data/master-template.xlsx
@@ -848,9 +848,6 @@
     <t>Western blot</t>
   </si>
   <si>
-    <t>Associated Assay metdata</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -915,6 +912,9 @@
   </si>
   <si>
     <t>Powered by:</t>
+  </si>
+  <si>
+    <t>Associated Assay</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1714,7 @@
   <dimension ref="A2:AMJ19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1730,11 +1730,11 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C2" s="11"/>
       <c r="E2" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C4" s="6"/>
       <c r="E4" s="28"/>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="5" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
@@ -1796,7 +1796,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="E7" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="C8" s="13"/>
       <c r="E8" s="21"/>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" s="5"/>
       <c r="E11" s="20"/>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C12" s="15"/>
       <c r="E12" s="20"/>
@@ -1870,38 +1870,38 @@
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>1</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2015,7 +2015,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3267,7 +3267,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>